<commit_message>
end of day dump
</commit_message>
<xml_diff>
--- a/cluster to pathway.xlsx
+++ b/cluster to pathway.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>lens fiber cell differentiation</t>
   </si>
@@ -142,6 +142,30 @@
   </si>
   <si>
     <t>(juvenile cataract)</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>theory 1: retention of galactitol in the lens leads to osmotic swelling; this results in increased lens permeability and loss of amino acids, and later fiber cell lysis and vacoule formation. Theory 2: Autoxidation of galactose results in ROS (H2O2). Also mentions depletion of NADPH, GSH, ATP...</t>
+  </si>
+  <si>
+    <t>myoblast fusion is associated with calpain</t>
+  </si>
+  <si>
+    <t>ascorbic acid is an antioxidant, and is found in decreased levels in cataracteous lenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pentose phosphate pathway regenerates NADPH. </t>
+  </si>
+  <si>
+    <t>mutation or deletion of Ncoa6 gene results in cataract</t>
+  </si>
+  <si>
+    <t>"ectopic activation of Wnt/b-catenin signaling in lens fiber cells using a transgenic mouse model results in aberrant lens fiber cell differentiation and cataract formation"</t>
+  </si>
+  <si>
+    <t>various hereditary disorders result in genetic cataract</t>
   </si>
 </sst>
 </file>
@@ -468,59 +492,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -528,31 +556,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -560,129 +588,150 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:B21">
-    <sortCondition ref="A2:A21"/>
+  <sortState ref="A2:E25">
+    <sortCondition ref="B2:B25"/>
   </sortState>
   <conditionalFormatting sqref="A1:A25">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
all important files in one folder
</commit_message>
<xml_diff>
--- a/cluster to pathway.xlsx
+++ b/cluster to pathway.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>lens fiber cell differentiation</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>various hereditary disorders result in genetic cataract</t>
+  </si>
+  <si>
+    <t>(?)</t>
+  </si>
+  <si>
+    <t>(Pierson syndrome)</t>
   </si>
 </sst>
 </file>
@@ -208,7 +214,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -495,7 +508,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +659,9 @@
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -697,6 +713,12 @@
       </c>
       <c r="B22" t="s">
         <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -734,7 +756,7 @@
     <sortCondition ref="B2:B25"/>
   </sortState>
   <conditionalFormatting sqref="A1:A25">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>